<commit_message>
added Log-info to TC001-TC026
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Fruits</t>
   </si>
@@ -200,6 +200,33 @@
   </si>
   <si>
     <t>RandomPassword: JPGAdrbLRandomEmail: XXjhVk@gmailAccountDeleted</t>
+  </si>
+  <si>
+    <t>RandomPassword: Jz3lln4lRandomEmail: fPOojO@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: Jz3lln4lRandomEmail: fPOojO@gmailAccountDeleted</t>
+  </si>
+  <si>
+    <t>RandomPassword: Ii5D9eczRandomEmail: SaBhRE@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: eeNScyHARandomEmail: stFpeZ@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: eeNScyHARandomEmail: stFpeZ@gmailAccountDeleted</t>
+  </si>
+  <si>
+    <t>RandomPassword: sN2rpGmNRandomEmail: cKOBky@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: sN2rpGmNRandomEmail: cKOBky@gmailAccountDeleted</t>
+  </si>
+  <si>
+    <t>RandomPassword: yDqo2EK5RandomEmail: PbQBjI@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: b8HuVog2RandomEmail: LzWZfY@gmailAccountCreated</t>
   </si>
 </sst>
 </file>
@@ -532,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A700" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -864,6 +891,51 @@
         <v>61</v>
       </c>
     </row>
+    <row r="62">
+      <c r="C62" t="s" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="C63" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" t="s" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="C65" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="C67" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="C69" t="s" s="0">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" t="s" s="0">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update Error info TC001-TC026
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Fruits</t>
   </si>
@@ -227,6 +227,27 @@
   </si>
   <si>
     <t>RandomPassword: b8HuVog2RandomEmail: LzWZfY@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: DyFbkobqRandomEmail: rMETeA@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: DyFbkobqRandomEmail: rMETeA@gmailAccountDeleted</t>
+  </si>
+  <si>
+    <t>RandomPassword: hhoSOq2oRandomEmail: zymyvx@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: Rl5D7YakRandomEmail: YkvChS@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: AQ8BNTt2RandomEmail: wLHFlN@gmailAccountCreated</t>
+  </si>
+  <si>
+    <t>RandomPassword: AQ8BNTt2RandomEmail: wLHFlN@gmailAccountDeleted</t>
+  </si>
+  <si>
+    <t>RandomPassword: lhWAs14ERandomEmail: XHKQrv@gmailAccountCreated</t>
   </si>
 </sst>
 </file>
@@ -559,7 +580,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A700" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -936,6 +957,41 @@
         <v>70</v>
       </c>
     </row>
+    <row r="71">
+      <c r="C71" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="C72" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="C73" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="C75" t="s" s="0">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="C77" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>